<commit_message>
Fix package for C15, C20, C21, C22 on schematic and on BOM.  PCB footprints were already correct
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex BOM.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4041FF-79F0-474E-B646-F4A83039C217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="29925" yWindow="1020" windowWidth="24165" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="DK Order" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="253">
   <si>
     <t>Qty</t>
   </si>
@@ -143,9 +149,6 @@
     <t>490-14306-1-ND</t>
   </si>
   <si>
-    <t>GRM155R61A475MEAAD</t>
-  </si>
-  <si>
     <t>C19</t>
   </si>
   <si>
@@ -167,9 +170,6 @@
     <t>445-7592-1-ND</t>
   </si>
   <si>
-    <t>C2012X7R1A106M125AC</t>
-  </si>
-  <si>
     <t>C23</t>
   </si>
   <si>
@@ -224,9 +224,6 @@
     <t>SK310A-LTPMSCT-ND</t>
   </si>
   <si>
-    <t>迪一</t>
-  </si>
-  <si>
     <t>SK310A-LTP</t>
   </si>
   <si>
@@ -768,13 +765,28 @@
   </si>
   <si>
     <t>SC32S-7PF20PPM</t>
+  </si>
+  <si>
+    <t>490-14466-1-ND</t>
+  </si>
+  <si>
+    <t>GRM21BR71C475KE51L</t>
+  </si>
+  <si>
+    <t>1276-6641-1-ND</t>
+  </si>
+  <si>
+    <t>CL31B106MOHNNNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,22 +829,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -870,7 +891,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -904,6 +925,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -938,9 +960,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1113,19 +1136,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="6" width="30.7109375" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1165,7 +1190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1182,7 +1207,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1202,7 +1227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>101</v>
       </c>
@@ -1219,7 +1244,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1236,7 +1261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1253,7 +1278,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1270,7 +1295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1287,7 +1312,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>28</v>
       </c>
@@ -1304,7 +1329,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1315,463 +1340,469 @@
         <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>45</v>
       </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
       <c r="D13" t="s">
+        <v>250</v>
+      </c>
+      <c r="E13" t="s">
+        <v>252</v>
+      </c>
+      <c r="F13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="F13" t="s">
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="F14" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
         <v>54</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>55</v>
       </c>
-      <c r="D15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
         <v>58</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="s">
         <v>59</v>
       </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
         <v>62</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>63</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="F17" t="s">
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>66</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
+        <v>252</v>
+      </c>
+      <c r="F18" t="s">
         <v>67</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>68</v>
       </c>
-      <c r="E18" t="s">
+      <c r="C19" t="s">
         <v>69</v>
       </c>
-      <c r="F18" t="s">
+      <c r="D19" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="F19" t="s">
         <v>71</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
         <v>72</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C20" t="s">
         <v>73</v>
       </c>
-      <c r="F19" t="s">
+      <c r="D20" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="F20" t="s">
         <v>75</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
         <v>76</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C21" t="s">
         <v>77</v>
       </c>
-      <c r="F20" t="s">
+      <c r="D21" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="F21" t="s">
         <v>79</v>
       </c>
-      <c r="C21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" t="s">
         <v>83</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>84</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
         <v>85</v>
       </c>
-      <c r="F22" t="s">
+      <c r="D23" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="F23" t="s">
         <v>87</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
         <v>88</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C24" t="s">
         <v>89</v>
       </c>
-      <c r="F23" t="s">
+      <c r="D24" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="F24" t="s">
         <v>91</v>
       </c>
-      <c r="C24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
         <v>98</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>99</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>100</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
         <v>101</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>102</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>103</v>
       </c>
-      <c r="F27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="F28" t="s">
         <v>104</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
         <v>105</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C29" t="s">
         <v>106</v>
       </c>
-      <c r="F28" t="s">
+      <c r="D29" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="F29" t="s">
         <v>108</v>
       </c>
-      <c r="C29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" t="s">
         <v>112</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
         <v>113</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C31" t="s">
         <v>114</v>
       </c>
-      <c r="F30" t="s">
+      <c r="D31" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="F31" t="s">
         <v>116</v>
       </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
         <v>117</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C32" t="s">
         <v>118</v>
       </c>
-      <c r="F31" t="s">
+      <c r="D32" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="F32" t="s">
         <v>120</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
         <v>121</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C33" t="s">
         <v>122</v>
       </c>
-      <c r="F32" t="s">
+      <c r="D33" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="F33" t="s">
         <v>124</v>
       </c>
-      <c r="C33" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" t="s">
-        <v>126</v>
-      </c>
-      <c r="F33" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
       <c r="B34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" t="s">
         <v>128</v>
       </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
         <v>129</v>
       </c>
-      <c r="D34" t="s">
+      <c r="C35" t="s">
         <v>130</v>
       </c>
-      <c r="F34" t="s">
+      <c r="D35" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="F35" t="s">
         <v>132</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
         <v>133</v>
       </c>
-      <c r="D35" t="s">
+      <c r="C36" t="s">
         <v>134</v>
       </c>
-      <c r="F35" t="s">
+      <c r="D36" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="F36" t="s">
         <v>136</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
         <v>137</v>
       </c>
-      <c r="D36" t="s">
+      <c r="C37" t="s">
         <v>138</v>
       </c>
-      <c r="F36" t="s">
+      <c r="D37" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="F37" t="s">
         <v>140</v>
       </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
         <v>141</v>
-      </c>
-      <c r="D37" t="s">
-        <v>142</v>
-      </c>
-      <c r="F37" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>144</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
@@ -1780,516 +1811,516 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" t="s">
+        <v>144</v>
+      </c>
+      <c r="F39" t="s">
         <v>145</v>
       </c>
-      <c r="C39" t="s">
-        <v>146</v>
-      </c>
-      <c r="D39" t="s">
-        <v>147</v>
-      </c>
-      <c r="F39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>20</v>
       </c>
       <c r="B40" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" t="s">
+        <v>148</v>
+      </c>
+      <c r="F40" t="s">
         <v>149</v>
       </c>
-      <c r="C40" t="s">
-        <v>150</v>
-      </c>
-      <c r="D40" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>20</v>
       </c>
       <c r="B41" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" t="s">
+        <v>151</v>
+      </c>
+      <c r="D41" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" t="s">
         <v>153</v>
       </c>
-      <c r="C41" t="s">
-        <v>154</v>
-      </c>
-      <c r="D41" t="s">
-        <v>155</v>
-      </c>
-      <c r="F41" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
       <c r="B42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" t="s">
+        <v>156</v>
+      </c>
+      <c r="F42" t="s">
         <v>157</v>
       </c>
-      <c r="C42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D42" t="s">
-        <v>159</v>
-      </c>
-      <c r="F42" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
       <c r="B43" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" t="s">
         <v>161</v>
       </c>
-      <c r="C43" t="s">
-        <v>162</v>
-      </c>
-      <c r="D43" t="s">
-        <v>163</v>
-      </c>
-      <c r="F43" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C44" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D44" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
       <c r="B45" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" t="s">
+        <v>165</v>
+      </c>
+      <c r="F45" t="s">
         <v>166</v>
       </c>
-      <c r="C45" t="s">
-        <v>167</v>
-      </c>
-      <c r="D45" t="s">
-        <v>168</v>
-      </c>
-      <c r="F45" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
       <c r="B46" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" t="s">
+        <v>169</v>
+      </c>
+      <c r="F46" t="s">
         <v>170</v>
       </c>
-      <c r="C46" t="s">
-        <v>171</v>
-      </c>
-      <c r="D46" t="s">
-        <v>172</v>
-      </c>
-      <c r="F46" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
       <c r="B47" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" t="s">
+        <v>172</v>
+      </c>
+      <c r="D47" t="s">
+        <v>173</v>
+      </c>
+      <c r="F47" t="s">
         <v>174</v>
       </c>
-      <c r="C47" t="s">
-        <v>175</v>
-      </c>
-      <c r="D47" t="s">
-        <v>176</v>
-      </c>
-      <c r="F47" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>6</v>
       </c>
       <c r="B48" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" t="s">
+        <v>176</v>
+      </c>
+      <c r="D48" t="s">
+        <v>177</v>
+      </c>
+      <c r="F48" t="s">
         <v>178</v>
       </c>
-      <c r="C48" t="s">
-        <v>179</v>
-      </c>
-      <c r="D48" t="s">
-        <v>180</v>
-      </c>
-      <c r="F48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6</v>
       </c>
       <c r="B49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" t="s">
+        <v>181</v>
+      </c>
+      <c r="F49" t="s">
         <v>182</v>
       </c>
-      <c r="C49" t="s">
-        <v>183</v>
-      </c>
-      <c r="D49" t="s">
-        <v>184</v>
-      </c>
-      <c r="F49" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2</v>
       </c>
       <c r="B50" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" t="s">
+        <v>185</v>
+      </c>
+      <c r="E50" t="s">
         <v>186</v>
       </c>
-      <c r="C50" t="s">
+      <c r="F50" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
         <v>187</v>
       </c>
-      <c r="D50" t="s">
+      <c r="C51" t="s">
         <v>188</v>
       </c>
-      <c r="E50" t="s">
+      <c r="D51" t="s">
         <v>189</v>
       </c>
-      <c r="F50" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51">
-        <v>1</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="F51" t="s">
         <v>190</v>
       </c>
-      <c r="C51" t="s">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
         <v>191</v>
       </c>
-      <c r="D51" t="s">
+      <c r="C52" t="s">
         <v>192</v>
       </c>
-      <c r="F51" t="s">
+      <c r="D52" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="F52" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
         <v>194</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>195</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>196</v>
       </c>
-      <c r="F52" t="s">
+      <c r="E53" t="s">
+        <v>197</v>
+      </c>
+      <c r="F53" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53" t="s">
-        <v>197</v>
-      </c>
-      <c r="C53" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
         <v>198</v>
       </c>
-      <c r="D53" t="s">
+      <c r="C54" t="s">
         <v>199</v>
       </c>
-      <c r="E53" t="s">
+      <c r="D54" t="s">
         <v>200</v>
       </c>
-      <c r="F53" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="F54" t="s">
         <v>201</v>
       </c>
-      <c r="C54" t="s">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
         <v>202</v>
       </c>
-      <c r="D54" t="s">
+      <c r="C55" t="s">
         <v>203</v>
       </c>
-      <c r="F54" t="s">
+      <c r="D55" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55">
-        <v>1</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="F55" t="s">
         <v>205</v>
       </c>
-      <c r="C55" t="s">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
         <v>206</v>
       </c>
-      <c r="D55" t="s">
+      <c r="C56" t="s">
         <v>207</v>
       </c>
-      <c r="F55" t="s">
+      <c r="D56" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56">
-        <v>1</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="F56" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
         <v>209</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>210</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>211</v>
       </c>
-      <c r="F56" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57">
-        <v>1</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="F57" t="s">
         <v>212</v>
       </c>
-      <c r="C57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D57" t="s">
-        <v>214</v>
-      </c>
-      <c r="F57" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3</v>
       </c>
       <c r="B58" t="s">
+        <v>213</v>
+      </c>
+      <c r="C58" t="s">
+        <v>214</v>
+      </c>
+      <c r="D58" t="s">
+        <v>215</v>
+      </c>
+      <c r="F58" t="s">
         <v>216</v>
       </c>
-      <c r="C58" t="s">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
         <v>217</v>
       </c>
-      <c r="D58" t="s">
+      <c r="C59" t="s">
         <v>218</v>
       </c>
-      <c r="F58" t="s">
+      <c r="D59" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="F59" t="s">
         <v>220</v>
       </c>
-      <c r="C59" t="s">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
         <v>221</v>
       </c>
-      <c r="D59" t="s">
+      <c r="C60" t="s">
         <v>222</v>
       </c>
-      <c r="F59" t="s">
+      <c r="D60" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60">
-        <v>1</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="F60" t="s">
         <v>224</v>
       </c>
-      <c r="C60" t="s">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
         <v>225</v>
       </c>
-      <c r="D60" t="s">
+      <c r="C61" t="s">
+        <v>222</v>
+      </c>
+      <c r="D61" t="s">
+        <v>223</v>
+      </c>
+      <c r="F61" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
         <v>226</v>
       </c>
-      <c r="F60" t="s">
+      <c r="C62" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61">
-        <v>1</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="D62" t="s">
         <v>228</v>
       </c>
-      <c r="C61" t="s">
-        <v>225</v>
-      </c>
-      <c r="D61" t="s">
-        <v>226</v>
-      </c>
-      <c r="F61" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62">
-        <v>1</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="F62" t="s">
         <v>229</v>
       </c>
-      <c r="C62" t="s">
-        <v>230</v>
-      </c>
-      <c r="D62" t="s">
-        <v>231</v>
-      </c>
-      <c r="F62" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C63" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>6</v>
       </c>
       <c r="B64" t="s">
+        <v>232</v>
+      </c>
+      <c r="C64" t="s">
+        <v>233</v>
+      </c>
+      <c r="D64" t="s">
+        <v>234</v>
+      </c>
+      <c r="F64" t="s">
         <v>235</v>
       </c>
-      <c r="C64" t="s">
-        <v>236</v>
-      </c>
-      <c r="D64" t="s">
-        <v>237</v>
-      </c>
-      <c r="F64" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C65" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2</v>
       </c>
       <c r="B66" t="s">
+        <v>237</v>
+      </c>
+      <c r="C66" t="s">
+        <v>238</v>
+      </c>
+      <c r="D66" t="s">
+        <v>239</v>
+      </c>
+      <c r="F66" t="s">
         <v>240</v>
       </c>
-      <c r="C66" t="s">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
         <v>241</v>
       </c>
-      <c r="D66" t="s">
+      <c r="C67" t="s">
         <v>242</v>
       </c>
-      <c r="F66" t="s">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67">
-        <v>1</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="C68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
         <v>244</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C69" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68">
-        <v>1</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="D69" t="s">
         <v>246</v>
       </c>
-      <c r="C68" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69">
-        <v>1</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="F69" t="s">
         <v>247</v>
-      </c>
-      <c r="C69" t="s">
-        <v>248</v>
-      </c>
-      <c r="D69" t="s">
-        <v>249</v>
-      </c>
-      <c r="F69" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2298,18 +2329,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2320,7 +2351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2331,7 +2362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2342,7 +2373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>101</v>
       </c>
@@ -2353,7 +2384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2364,7 +2395,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2375,7 +2406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2386,7 +2417,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2397,7 +2428,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>28</v>
       </c>
@@ -2408,7 +2439,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2419,608 +2450,608 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
       <c r="C13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
         <v>62</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>66</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>71</v>
-      </c>
       <c r="C18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
         <v>98</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
         <v>101</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C35" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>145</v>
-      </c>
       <c r="C37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C38" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C42" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C43" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C44" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C46" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C47" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C48" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
       <c r="B49" t="s">
+        <v>191</v>
+      </c>
+      <c r="C49" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
         <v>194</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
-        <v>197</v>
-      </c>
-      <c r="C50" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C51" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C52" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
       <c r="B53" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
         <v>209</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
-        <v>212</v>
-      </c>
-      <c r="C54" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C55" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C56" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C57" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>225</v>
+      </c>
+      <c r="C58" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C59" t="s">
         <v>228</v>
       </c>
-      <c r="C58" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s">
-        <v>229</v>
-      </c>
-      <c r="C59" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C61" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C63" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1</v>
       </c>
       <c r="B64" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65">
-        <v>1</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C66" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66">
-        <v>1</v>
-      </c>
-      <c r="B66" t="s">
-        <v>247</v>
-      </c>
-      <c r="C66" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change R5 to DNP on schematic and BOM
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4041FF-79F0-474E-B646-F4A83039C217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551B994B-FD4D-467C-BC7B-F4A21D95E5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="1020" windowWidth="24165" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="900" windowWidth="24165" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="253">
   <si>
     <t>Qty</t>
   </si>
@@ -1139,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1437,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1710,6 +1710,9 @@
       </c>
       <c r="F32" t="s">
         <v>120</v>
+      </c>
+      <c r="G32" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change 1 ohm power resistors to 2 watt parts, changed schematic and BOM
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551B994B-FD4D-467C-BC7B-F4A21D95E5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BCEF65-0F1A-4D61-BFF8-DACEC9343D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="900" windowWidth="24165" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1830" yWindow="1005" windowWidth="24165" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="254">
   <si>
     <t>Qty</t>
   </si>
@@ -563,15 +563,9 @@
     <t>R34, R35, R62, R68, R98, R99</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>118-CR2512-F/-1R00ELFCT-ND</t>
   </si>
   <si>
-    <t>CR2512-F/-1R00ELF</t>
-  </si>
-  <si>
     <t>SW1, SW2</t>
   </si>
   <si>
@@ -780,6 +774,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1R 2W</t>
+  </si>
+  <si>
+    <t>CRM2512-JW-1R0ELFCT-ND</t>
+  </si>
+  <si>
+    <t>CRM2512-JW-1R0ELF</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,13 +1343,13 @@
         <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1377,13 +1380,13 @@
         <v>47</v>
       </c>
       <c r="D13" t="s">
+        <v>248</v>
+      </c>
+      <c r="E13" t="s">
         <v>250</v>
       </c>
-      <c r="E13" t="s">
-        <v>252</v>
-      </c>
       <c r="F13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1468,7 +1471,7 @@
         <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F18" t="s">
         <v>67</v>
@@ -1995,13 +1998,13 @@
         <v>179</v>
       </c>
       <c r="C49" t="s">
-        <v>180</v>
+        <v>251</v>
       </c>
       <c r="D49" t="s">
-        <v>181</v>
+        <v>252</v>
       </c>
       <c r="F49" t="s">
-        <v>182</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2009,19 +2012,19 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" t="s">
+        <v>182</v>
+      </c>
+      <c r="D50" t="s">
         <v>183</v>
       </c>
-      <c r="C50" t="s">
+      <c r="E50" t="s">
         <v>184</v>
       </c>
-      <c r="D50" t="s">
-        <v>185</v>
-      </c>
-      <c r="E50" t="s">
-        <v>186</v>
-      </c>
       <c r="F50" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2029,16 +2032,16 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" t="s">
+        <v>186</v>
+      </c>
+      <c r="D51" t="s">
         <v>187</v>
       </c>
-      <c r="C51" t="s">
+      <c r="F51" t="s">
         <v>188</v>
-      </c>
-      <c r="D51" t="s">
-        <v>189</v>
-      </c>
-      <c r="F51" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2046,16 +2049,16 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" t="s">
+        <v>190</v>
+      </c>
+      <c r="D52" t="s">
         <v>191</v>
       </c>
-      <c r="C52" t="s">
-        <v>192</v>
-      </c>
-      <c r="D52" t="s">
-        <v>193</v>
-      </c>
       <c r="F52" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2063,19 +2066,19 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
+        <v>192</v>
+      </c>
+      <c r="C53" t="s">
+        <v>193</v>
+      </c>
+      <c r="D53" t="s">
         <v>194</v>
       </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
         <v>195</v>
       </c>
-      <c r="D53" t="s">
-        <v>196</v>
-      </c>
-      <c r="E53" t="s">
-        <v>197</v>
-      </c>
       <c r="F53" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2083,16 +2086,16 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
+        <v>196</v>
+      </c>
+      <c r="C54" t="s">
+        <v>197</v>
+      </c>
+      <c r="D54" t="s">
         <v>198</v>
       </c>
-      <c r="C54" t="s">
+      <c r="F54" t="s">
         <v>199</v>
-      </c>
-      <c r="D54" t="s">
-        <v>200</v>
-      </c>
-      <c r="F54" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2100,16 +2103,16 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
+        <v>200</v>
+      </c>
+      <c r="C55" t="s">
+        <v>201</v>
+      </c>
+      <c r="D55" t="s">
         <v>202</v>
       </c>
-      <c r="C55" t="s">
+      <c r="F55" t="s">
         <v>203</v>
-      </c>
-      <c r="D55" t="s">
-        <v>204</v>
-      </c>
-      <c r="F55" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2117,16 +2120,16 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
+        <v>204</v>
+      </c>
+      <c r="C56" t="s">
+        <v>205</v>
+      </c>
+      <c r="D56" t="s">
         <v>206</v>
       </c>
-      <c r="C56" t="s">
-        <v>207</v>
-      </c>
-      <c r="D56" t="s">
-        <v>208</v>
-      </c>
       <c r="F56" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2134,16 +2137,16 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
+        <v>207</v>
+      </c>
+      <c r="C57" t="s">
+        <v>208</v>
+      </c>
+      <c r="D57" t="s">
         <v>209</v>
       </c>
-      <c r="C57" t="s">
+      <c r="F57" t="s">
         <v>210</v>
-      </c>
-      <c r="D57" t="s">
-        <v>211</v>
-      </c>
-      <c r="F57" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2151,16 +2154,16 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
+        <v>211</v>
+      </c>
+      <c r="C58" t="s">
+        <v>212</v>
+      </c>
+      <c r="D58" t="s">
         <v>213</v>
       </c>
-      <c r="C58" t="s">
+      <c r="F58" t="s">
         <v>214</v>
-      </c>
-      <c r="D58" t="s">
-        <v>215</v>
-      </c>
-      <c r="F58" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2168,16 +2171,16 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
+        <v>215</v>
+      </c>
+      <c r="C59" t="s">
+        <v>216</v>
+      </c>
+      <c r="D59" t="s">
         <v>217</v>
       </c>
-      <c r="C59" t="s">
+      <c r="F59" t="s">
         <v>218</v>
-      </c>
-      <c r="D59" t="s">
-        <v>219</v>
-      </c>
-      <c r="F59" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2185,16 +2188,16 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
+        <v>219</v>
+      </c>
+      <c r="C60" t="s">
+        <v>220</v>
+      </c>
+      <c r="D60" t="s">
         <v>221</v>
       </c>
-      <c r="C60" t="s">
+      <c r="F60" t="s">
         <v>222</v>
-      </c>
-      <c r="D60" t="s">
-        <v>223</v>
-      </c>
-      <c r="F60" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2202,16 +2205,16 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C61" t="s">
+        <v>220</v>
+      </c>
+      <c r="D61" t="s">
+        <v>221</v>
+      </c>
+      <c r="F61" t="s">
         <v>222</v>
-      </c>
-      <c r="D61" t="s">
-        <v>223</v>
-      </c>
-      <c r="F61" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2219,16 +2222,16 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
+        <v>224</v>
+      </c>
+      <c r="C62" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" t="s">
         <v>226</v>
       </c>
-      <c r="C62" t="s">
+      <c r="F62" t="s">
         <v>227</v>
-      </c>
-      <c r="D62" t="s">
-        <v>228</v>
-      </c>
-      <c r="F62" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2236,10 +2239,10 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C63" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2247,16 +2250,16 @@
         <v>6</v>
       </c>
       <c r="B64" t="s">
+        <v>230</v>
+      </c>
+      <c r="C64" t="s">
+        <v>231</v>
+      </c>
+      <c r="D64" t="s">
         <v>232</v>
       </c>
-      <c r="C64" t="s">
+      <c r="F64" t="s">
         <v>233</v>
-      </c>
-      <c r="D64" t="s">
-        <v>234</v>
-      </c>
-      <c r="F64" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2264,10 +2267,10 @@
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C65" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2275,16 +2278,16 @@
         <v>2</v>
       </c>
       <c r="B66" t="s">
+        <v>235</v>
+      </c>
+      <c r="C66" t="s">
+        <v>236</v>
+      </c>
+      <c r="D66" t="s">
         <v>237</v>
       </c>
-      <c r="C66" t="s">
+      <c r="F66" t="s">
         <v>238</v>
-      </c>
-      <c r="D66" t="s">
-        <v>239</v>
-      </c>
-      <c r="F66" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2292,10 +2295,10 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C67" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2303,10 +2306,10 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C68" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2314,16 +2317,16 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
+        <v>242</v>
+      </c>
+      <c r="C69" t="s">
+        <v>243</v>
+      </c>
+      <c r="D69" t="s">
         <v>244</v>
       </c>
-      <c r="C69" t="s">
+      <c r="F69" t="s">
         <v>245</v>
-      </c>
-      <c r="D69" t="s">
-        <v>246</v>
-      </c>
-      <c r="F69" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2846,7 +2849,7 @@
         <v>179</v>
       </c>
       <c r="C46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2854,10 +2857,10 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
+        <v>181</v>
+      </c>
+      <c r="C47" t="s">
         <v>183</v>
-      </c>
-      <c r="C47" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2865,10 +2868,10 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" t="s">
         <v>187</v>
-      </c>
-      <c r="C48" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2876,10 +2879,10 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" t="s">
         <v>191</v>
-      </c>
-      <c r="C49" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2887,10 +2890,10 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" t="s">
         <v>194</v>
-      </c>
-      <c r="C50" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2898,10 +2901,10 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
+        <v>196</v>
+      </c>
+      <c r="C51" t="s">
         <v>198</v>
-      </c>
-      <c r="C51" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2909,10 +2912,10 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
+        <v>200</v>
+      </c>
+      <c r="C52" t="s">
         <v>202</v>
-      </c>
-      <c r="C52" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2920,10 +2923,10 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
+        <v>204</v>
+      </c>
+      <c r="C53" t="s">
         <v>206</v>
-      </c>
-      <c r="C53" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2931,10 +2934,10 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
+        <v>207</v>
+      </c>
+      <c r="C54" t="s">
         <v>209</v>
-      </c>
-      <c r="C54" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2942,10 +2945,10 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
+        <v>211</v>
+      </c>
+      <c r="C55" t="s">
         <v>213</v>
-      </c>
-      <c r="C55" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2953,10 +2956,10 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
+        <v>215</v>
+      </c>
+      <c r="C56" t="s">
         <v>217</v>
-      </c>
-      <c r="C56" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2964,10 +2967,10 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" t="s">
         <v>221</v>
-      </c>
-      <c r="C57" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2975,10 +2978,10 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C58" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2986,10 +2989,10 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
+        <v>224</v>
+      </c>
+      <c r="C59" t="s">
         <v>226</v>
-      </c>
-      <c r="C59" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2997,7 +3000,7 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3005,10 +3008,10 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
+        <v>230</v>
+      </c>
+      <c r="C61" t="s">
         <v>232</v>
-      </c>
-      <c r="C61" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3016,7 +3019,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3024,10 +3027,10 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
+        <v>235</v>
+      </c>
+      <c r="C63" t="s">
         <v>237</v>
-      </c>
-      <c r="C63" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3035,7 +3038,7 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -3043,7 +3046,7 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3051,10 +3054,10 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
+        <v>242</v>
+      </c>
+      <c r="C66" t="s">
         <v>244</v>
-      </c>
-      <c r="C66" t="s">
-        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>